<commit_message>
MAJ pins carte avant
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Carte avant/Pin Carte Avant.xlsx
+++ b/EL - Electrical/Autre/Carte avant/Pin Carte Avant.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732C0DFB-7E06-4DB5-B0F5-AF625C8545F6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>GND</t>
   </si>
@@ -128,12 +127,15 @@
   </si>
   <si>
     <t>N_PIN</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -175,11 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,7 +226,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55129FAB-B89E-42C3-997C-596B13A4DE44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55129FAB-B89E-42C3-997C-596B13A4DE44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -304,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -339,7 +348,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -516,24 +525,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -557,6 +566,9 @@
       </c>
     </row>
     <row r="4" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="Q4" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="U4" t="s">
         <v>31</v>
       </c>
@@ -606,10 +618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>18</v>
       </c>
@@ -623,10 +632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,7 +640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>0</v>
       </c>
@@ -645,7 +651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>7</v>
       </c>
@@ -656,39 +662,42 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="L21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>8</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L24" s="3">
         <v>3</v>
       </c>
-      <c r="N24" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>11</v>
       </c>
@@ -699,21 +708,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="L26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>23</v>
       </c>
@@ -724,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
       <c r="G31" s="1" t="s">
         <v>4</v>
       </c>
@@ -735,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
       <c r="G32" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
modif pin carte avant
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Carte avant/Pin Carte Avant.xlsx
+++ b/EL - Electrical/Autre/Carte avant/Pin Carte Avant.xlsx
@@ -3,30 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903250AB-CA29-4627-9B4A-592786C1296E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C73DEA-B12F-4B0E-9EB9-88FCF406F4B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>GND</t>
   </si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Error_motored</t>
   </si>
 </sst>
 </file>
@@ -280,8 +280,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>591659</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>6551</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>135255</xdr:rowOff>
     </xdr:to>
@@ -597,63 +597,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:U32"/>
+  <dimension ref="C2:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:21" x14ac:dyDescent="0.25">
       <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="Q3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="Q4" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="Q5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="Q6" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="Q7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="U9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="L13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E14" s="3" t="s">
         <v>3</v>
       </c>
@@ -661,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
@@ -685,8 +685,11 @@
       <c r="L16" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
         <v>18</v>
@@ -701,7 +704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
       <c r="E18" s="10" t="s">
         <v>0</v>
@@ -709,8 +712,11 @@
       <c r="L18" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N18" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E19" s="3" t="s">
         <v>0</v>
       </c>
@@ -723,11 +729,8 @@
       <c r="N19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O19" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
@@ -740,11 +743,8 @@
       <c r="N20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O20" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="L21" s="10">
         <v>6</v>
@@ -752,8 +752,14 @@
       <c r="M21" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="T21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>9</v>
       </c>
@@ -764,7 +770,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D23" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>8</v>
       </c>
@@ -775,7 +784,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D24" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E24" s="3" t="s">
         <v>10</v>
       </c>
@@ -787,7 +799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E25" s="3" t="s">
         <v>11</v>
       </c>
@@ -798,7 +810,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
@@ -810,7 +822,7 @@
       </c>
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
         <v>23</v>
       </c>
@@ -821,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="G31" s="1" t="s">
         <v>4</v>
       </c>
@@ -832,7 +844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="G32" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,6 +853,11 @@
       </c>
       <c r="I32" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>